<commit_message>
Cambio de ciertos catches
</commit_message>
<xml_diff>
--- a/HojaControlAudicon.xlsx
+++ b/HojaControlAudicon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Escritorio\Audicon_FixedProcess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E602C3FD-908E-4511-8A1A-4DC49DEB0B19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E453E4-8809-410E-81B8-810893FB5D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="2355" windowWidth="18000" windowHeight="9375" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>